<commit_message>
Continuação da Implementação do importador de operações
</commit_message>
<xml_diff>
--- a/public/documentos/Importador.xlsx
+++ b/public/documentos/Importador.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="53">
   <si>
     <t>Login Usuário</t>
   </si>
@@ -62,30 +62,18 @@
     <t>29/10/2023</t>
   </si>
   <si>
-    <t>29/10/23</t>
-  </si>
-  <si>
-    <t>2023-10-29</t>
-  </si>
-  <si>
     <t>09:00</t>
   </si>
   <si>
     <t>09:15:23</t>
   </si>
   <si>
-    <t>09-12</t>
-  </si>
-  <si>
     <t>09:30</t>
   </si>
   <si>
     <t>09:40:23</t>
   </si>
   <si>
-    <t>09-15</t>
-  </si>
-  <si>
     <t>28/10/2023</t>
   </si>
   <si>
@@ -110,12 +98,6 @@
     <t>IZX-0000</t>
   </si>
   <si>
-    <t>IZX0000</t>
-  </si>
-  <si>
-    <t>IZX2829292</t>
-  </si>
-  <si>
     <t>02039741070</t>
   </si>
   <si>
@@ -149,9 +131,6 @@
     <t>11:00</t>
   </si>
   <si>
-    <t>IZX7H39</t>
-  </si>
-  <si>
     <t>III-9U99</t>
   </si>
   <si>
@@ -180,6 +159,30 @@
   </si>
   <si>
     <t>17:00</t>
+  </si>
+  <si>
+    <t>09:12</t>
+  </si>
+  <si>
+    <t>09:15</t>
+  </si>
+  <si>
+    <t>Descrição Veículo</t>
+  </si>
+  <si>
+    <t>Tipo do Veículo (Carro, Caminhão, Moto, Outro)</t>
+  </si>
+  <si>
+    <t>Nome Motorista</t>
+  </si>
+  <si>
+    <t>IZX-7H39</t>
+  </si>
+  <si>
+    <t>IZX-1000</t>
+  </si>
+  <si>
+    <t>IZX-2829</t>
   </si>
 </sst>
 </file>
@@ -525,11 +528,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -538,14 +541,16 @@
     <col min="2" max="2" width="13.54296875" style="4"/>
     <col min="3" max="3" width="15.81640625" style="4" customWidth="1"/>
     <col min="4" max="6" width="13.54296875" style="4"/>
-    <col min="7" max="7" width="21.453125" style="4" customWidth="1"/>
-    <col min="8" max="8" width="18.7265625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="18" style="4" customWidth="1"/>
-    <col min="10" max="11" width="20.54296875" style="4" customWidth="1"/>
-    <col min="12" max="16384" width="13.54296875" style="4"/>
+    <col min="7" max="7" width="23.54296875" style="4" customWidth="1"/>
+    <col min="8" max="8" width="23.81640625" style="4" customWidth="1"/>
+    <col min="9" max="10" width="21.453125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="18.7265625" style="4" customWidth="1"/>
+    <col min="12" max="12" width="18" style="4" customWidth="1"/>
+    <col min="13" max="14" width="20.54296875" style="4" customWidth="1"/>
+    <col min="15" max="16384" width="13.54296875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" s="3" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -565,260 +570,269 @@
         <v>10</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H2" s="4" t="s">
+      <c r="E6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>39</v>
+      <c r="E7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="4" t="s">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="H3" s="4" t="s">
+      <c r="E8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I8" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>34</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="J9" s="4" t="s">
-        <v>39</v>
+      <c r="K9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Continuação da Implementação do Importador
</commit_message>
<xml_diff>
--- a/public/documentos/Importador.xlsx
+++ b/public/documentos/Importador.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="64">
   <si>
     <t>Login Usuário</t>
   </si>
@@ -47,9 +47,6 @@
     <t>CPF Motorista (somente números)</t>
   </si>
   <si>
-    <t>Tipo (Normal/Emergência)</t>
-  </si>
-  <si>
     <t>Descrição Portaria (Entrada)</t>
   </si>
   <si>
@@ -125,9 +122,6 @@
     <t>Port</t>
   </si>
   <si>
-    <t>Normal</t>
-  </si>
-  <si>
     <t>11:00</t>
   </si>
   <si>
@@ -137,15 +131,6 @@
     <t>11192873949</t>
   </si>
   <si>
-    <t>Emergência</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
     <t>Teste</t>
   </si>
   <si>
@@ -155,9 +140,6 @@
     <t>16:00</t>
   </si>
   <si>
-    <t>E</t>
-  </si>
-  <si>
     <t>17:00</t>
   </si>
   <si>
@@ -183,6 +165,57 @@
   </si>
   <si>
     <t>IZX-2829</t>
+  </si>
+  <si>
+    <t>Kwid</t>
+  </si>
+  <si>
+    <t>Scania</t>
+  </si>
+  <si>
+    <t>Vectra</t>
+  </si>
+  <si>
+    <t>Titan 150</t>
+  </si>
+  <si>
+    <t>Volvo</t>
+  </si>
+  <si>
+    <t>Volks</t>
+  </si>
+  <si>
+    <t>Truck</t>
+  </si>
+  <si>
+    <t>carro</t>
+  </si>
+  <si>
+    <t>Carro</t>
+  </si>
+  <si>
+    <t>caminhão</t>
+  </si>
+  <si>
+    <t>Moto</t>
+  </si>
+  <si>
+    <t>Caminhão</t>
+  </si>
+  <si>
+    <t>Outro</t>
+  </si>
+  <si>
+    <t>CNPJ/CPF Empresa (somente números)</t>
+  </si>
+  <si>
+    <t>Nome da Empresa</t>
+  </si>
+  <si>
+    <t>Tipo Operação (Normal, Emergência)</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -238,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -248,6 +281,7 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -528,11 +562,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -543,14 +577,14 @@
     <col min="4" max="6" width="13.54296875" style="4"/>
     <col min="7" max="7" width="23.54296875" style="4" customWidth="1"/>
     <col min="8" max="8" width="23.81640625" style="4" customWidth="1"/>
-    <col min="9" max="10" width="21.453125" style="4" customWidth="1"/>
-    <col min="11" max="11" width="18.7265625" style="4" customWidth="1"/>
-    <col min="12" max="12" width="18" style="4" customWidth="1"/>
-    <col min="13" max="14" width="20.54296875" style="4" customWidth="1"/>
-    <col min="15" max="16384" width="13.54296875" style="4"/>
+    <col min="9" max="12" width="21.453125" style="4" customWidth="1"/>
+    <col min="13" max="13" width="18.7265625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="18" style="4" customWidth="1"/>
+    <col min="15" max="16" width="20.54296875" style="4" customWidth="1"/>
+    <col min="17" max="16384" width="13.54296875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="3" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" s="3" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -567,272 +601,304 @@
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="M2" s="4" t="s">
+      <c r="C5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="G7" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="4" t="s">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="K3" s="4" t="s">
+      <c r="F8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N9" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="L3" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>33</v>
-      </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="M6" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="M7" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="N7" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="M8" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="K9" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="L9" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="M9" s="4" t="s">
-        <v>33</v>
+    <row r="21" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F21" s="5" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>